<commit_message>
Updated Notebooks, sample excel sheets
</commit_message>
<xml_diff>
--- a/data_input/input_crop_TSUM_parameters_maiz_sugar.xlsx
+++ b/data_input/input_crop_TSUM_parameters_maiz_sugar.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Testing Gunther Data for Modification\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pyaez_github_test_env\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F262EC0-5A0F-411B-9804-BACA63B44B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F92754-0E04-41FE-968C-27441DB346FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-105" windowWidth="29040" windowHeight="15720" xr2:uid="{0EBC9278-16C4-4F19-BFBC-BE9217943952}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
   <si>
     <t>Crop_name</t>
   </si>
@@ -92,9 +92,6 @@
     <t>annual/perennial flag</t>
   </si>
   <si>
-    <t>maize_1_LUT_35</t>
-  </si>
-  <si>
     <t>HI</t>
   </si>
   <si>
@@ -153,6 +150,21 @@
   </si>
   <si>
     <t>low</t>
+  </si>
+  <si>
+    <t>maize</t>
+  </si>
+  <si>
+    <t>maiz49</t>
+  </si>
+  <si>
+    <t>min_cycle_len</t>
+  </si>
+  <si>
+    <t>max_cycle_len</t>
+  </si>
+  <si>
+    <t>height</t>
   </si>
 </sst>
 </file>
@@ -188,8 +200,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B29C5A6A-0B2F-4690-8ED4-94CA56D6CD01}">
-  <dimension ref="A1:AH3"/>
+  <dimension ref="A1:AK4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,25 +529,27 @@
     <col min="2" max="2" width="15.5703125" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="20.42578125" customWidth="1"/>
-    <col min="25" max="25" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.42578125" customWidth="1"/>
+    <col min="28" max="28" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
         <v>19</v>
-      </c>
-      <c r="D1" t="s">
-        <v>20</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -546,93 +561,102 @@
         <v>3</v>
       </c>
       <c r="H1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S1" t="s">
+        <v>11</v>
+      </c>
+      <c r="T1" t="s">
+        <v>12</v>
+      </c>
+      <c r="U1" t="s">
         <v>21</v>
       </c>
-      <c r="O1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1" t="s">
+      <c r="V1" t="s">
+        <v>13</v>
+      </c>
+      <c r="W1" t="s">
+        <v>14</v>
+      </c>
+      <c r="X1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB1" t="s">
         <v>22</v>
       </c>
-      <c r="S1" t="s">
-        <v>13</v>
-      </c>
-      <c r="T1" t="s">
-        <v>14</v>
-      </c>
-      <c r="U1" t="s">
-        <v>15</v>
-      </c>
-      <c r="V1" t="s">
-        <v>16</v>
-      </c>
-      <c r="W1" t="s">
-        <v>17</v>
-      </c>
-      <c r="X1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y1" t="s">
+      <c r="AC1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AD1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AE1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" t="s">
+      <c r="AF1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG1" t="s">
         <v>30</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AH1" t="s">
         <v>31</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AI1" t="s">
         <v>32</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AJ1" t="s">
         <v>33</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AK1" t="s">
         <v>34</v>
       </c>
-      <c r="AH1" t="s">
-        <v>35</v>
-      </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2">
         <v>0.45</v>
@@ -650,95 +674,104 @@
         <v>90</v>
       </c>
       <c r="H2">
+        <v>80</v>
+      </c>
+      <c r="I2">
+        <v>100</v>
+      </c>
+      <c r="J2">
         <v>0.3</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>1</v>
       </c>
-      <c r="J2">
-        <v>15</v>
-      </c>
-      <c r="K2">
-        <v>30</v>
-      </c>
       <c r="L2">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="M2">
         <v>15</v>
       </c>
       <c r="N2">
+        <v>30</v>
+      </c>
+      <c r="O2">
+        <v>40</v>
+      </c>
+      <c r="P2">
+        <v>15</v>
+      </c>
+      <c r="Q2">
         <v>0.3</v>
       </c>
-      <c r="O2">
+      <c r="R2">
         <v>1.2</v>
       </c>
-      <c r="P2">
+      <c r="S2">
         <v>0.35</v>
       </c>
-      <c r="Q2">
+      <c r="T2">
         <v>0.85</v>
       </c>
-      <c r="R2">
+      <c r="U2">
         <v>0.4</v>
       </c>
-      <c r="S2">
+      <c r="V2">
         <v>0.4</v>
       </c>
-      <c r="T2">
+      <c r="W2">
         <v>1.5</v>
       </c>
-      <c r="U2">
-        <v>0.5</v>
-      </c>
-      <c r="V2">
+      <c r="X2">
+        <v>0.2</v>
+      </c>
+      <c r="Y2">
         <v>1.25</v>
       </c>
-      <c r="W2">
+      <c r="Z2">
         <v>0</v>
       </c>
-      <c r="X2">
+      <c r="AA2">
         <v>15</v>
       </c>
-      <c r="Y2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>27</v>
-      </c>
       <c r="AB2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC2">
-        <f>AD2-(5%*AD2)</f>
-        <v>1140</v>
-      </c>
-      <c r="AD2">
-        <v>1200</v>
-      </c>
-      <c r="AE2">
+        <v>26</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF2">
+        <f>AG2-(5%*AG2)</f>
+        <v>1995</v>
+      </c>
+      <c r="AG2">
+        <v>2100</v>
+      </c>
+      <c r="AH2">
         <v>2300</v>
       </c>
-      <c r="AF2">
-        <f>AG2+(5% * AG2)</f>
+      <c r="AI2">
+        <f>AJ2+(5% * AJ2)</f>
         <v>3780</v>
       </c>
-      <c r="AG2">
+      <c r="AJ2">
         <v>3600</v>
       </c>
-      <c r="AH2">
+      <c r="AK2">
         <v>3150</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
         <v>37</v>
-      </c>
-      <c r="B3" t="s">
-        <v>38</v>
       </c>
       <c r="C3">
         <v>0.1</v>
@@ -756,97 +789,229 @@
         <v>330</v>
       </c>
       <c r="H3">
+        <v>150</v>
+      </c>
+      <c r="I3">
+        <v>360</v>
+      </c>
+      <c r="J3">
         <v>1.2</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>2</v>
       </c>
-      <c r="J3">
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3">
         <v>10</v>
       </c>
-      <c r="K3">
+      <c r="N3">
         <v>15</v>
       </c>
-      <c r="L3">
+      <c r="O3">
         <v>45</v>
       </c>
-      <c r="M3">
+      <c r="P3">
         <v>30</v>
       </c>
-      <c r="N3">
+      <c r="Q3">
         <v>0.4</v>
       </c>
-      <c r="O3">
+      <c r="R3">
         <v>1.25</v>
       </c>
-      <c r="P3">
+      <c r="S3">
         <v>0.75</v>
       </c>
-      <c r="Q3">
+      <c r="T3">
         <v>1</v>
       </c>
-      <c r="R3" t="s">
-        <v>27</v>
-      </c>
-      <c r="S3" t="s">
-        <v>27</v>
-      </c>
-      <c r="T3" t="s">
-        <v>27</v>
-      </c>
       <c r="U3" t="s">
-        <v>27</v>
-      </c>
-      <c r="V3">
+        <v>26</v>
+      </c>
+      <c r="V3" t="s">
+        <v>26</v>
+      </c>
+      <c r="W3" t="s">
+        <v>26</v>
+      </c>
+      <c r="X3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y3">
         <v>1.2</v>
       </c>
-      <c r="W3">
+      <c r="Z3">
         <v>1</v>
       </c>
-      <c r="X3">
+      <c r="AA3">
         <v>10</v>
       </c>
-      <c r="Y3">
+      <c r="AB3">
         <v>70</v>
       </c>
-      <c r="Z3">
+      <c r="AC3">
         <v>200</v>
       </c>
-      <c r="AA3">
+      <c r="AD3">
         <v>120</v>
       </c>
-      <c r="AB3">
+      <c r="AE3">
         <v>180</v>
       </c>
-      <c r="AC3">
-        <f>AD3-(5%*AD3)</f>
+      <c r="AF3">
+        <f>AG3-(5%*AG3)</f>
         <v>5700</v>
       </c>
-      <c r="AD3">
+      <c r="AG3">
         <v>6000</v>
       </c>
-      <c r="AE3">
+      <c r="AH3">
         <v>6750</v>
       </c>
-      <c r="AF3">
-        <f>AG3+(5% * AG3)</f>
-        <v>11497.5</v>
-      </c>
-      <c r="AG3">
+      <c r="AI3">
+        <v>11498</v>
+      </c>
+      <c r="AJ3">
         <v>10950</v>
       </c>
-      <c r="AH3">
+      <c r="AK3">
         <v>10000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4">
+        <v>0.45</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>135</v>
+      </c>
+      <c r="H4">
+        <v>115</v>
+      </c>
+      <c r="I4">
+        <v>155</v>
+      </c>
+      <c r="J4">
+        <v>0.3</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>3</v>
+      </c>
+      <c r="M4">
+        <v>20</v>
+      </c>
+      <c r="N4">
+        <v>30</v>
+      </c>
+      <c r="O4">
+        <v>35</v>
+      </c>
+      <c r="P4">
+        <v>15</v>
+      </c>
+      <c r="Q4">
+        <v>0.3</v>
+      </c>
+      <c r="R4">
+        <v>1.2</v>
+      </c>
+      <c r="S4">
+        <v>0.35</v>
+      </c>
+      <c r="T4">
+        <v>0.85</v>
+      </c>
+      <c r="U4">
+        <v>0.4</v>
+      </c>
+      <c r="V4">
+        <v>0.4</v>
+      </c>
+      <c r="W4">
+        <v>1.5</v>
+      </c>
+      <c r="X4">
+        <v>0.2</v>
+      </c>
+      <c r="Y4">
+        <v>1.25</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>10</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF4" s="1">
+        <f>ROUND(AG4-(5%*AG4),0)</f>
+        <v>2019</v>
+      </c>
+      <c r="AG4" s="1">
+        <v>2125</v>
+      </c>
+      <c r="AH4" s="1">
+        <v>2250</v>
+      </c>
+      <c r="AI4" s="1">
+        <v>4961</v>
+      </c>
+      <c r="AJ4" s="1">
+        <v>4725</v>
+      </c>
+      <c r="AK4" s="1">
+        <v>4050</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008864D41C708CC54AABC64DB9F8EC5160" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d21d14778ad924c5ebf493f4c28f6785">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="aecedfd1-a701-4d39-be9b-da32a8dfc2a5" xmlns:ns3="6cc8ca2e-56d8-406d-8e41-68c6b727753a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="76cfd8fd1da363887493d86d0c5919fe" ns2:_="" ns3:_="">
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008864D41C708CC54AABC64DB9F8EC5160" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8280e7c680d5d724f4413038ca100d1d">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="aecedfd1-a701-4d39-be9b-da32a8dfc2a5" xmlns:ns3="6cc8ca2e-56d8-406d-8e41-68c6b727753a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a78283ead66d0e44d8e1b525c3947135" ns2:_="" ns3:_="">
     <xsd:import namespace="aecedfd1-a701-4d39-be9b-da32a8dfc2a5"/>
     <xsd:import namespace="6cc8ca2e-56d8-406d-8e41-68c6b727753a"/>
     <xsd:element name="properties">
@@ -869,6 +1034,7 @@
                 <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -938,6 +1104,11 @@
     <xsd:element name="MediaLengthInSeconds" ma:index="22" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="23" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -1081,19 +1252,29 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55654B44-6725-4A31-9520-38E97C83B4A2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A77A2D2-FB5E-4D16-89FD-0C1B6E08F2B9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A77A2D2-FB5E-4D16-89FD-0C1B6E08F2B9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3494866B-24BB-495E-916D-2E3A591177B2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="aecedfd1-a701-4d39-be9b-da32a8dfc2a5"/>
+    <ds:schemaRef ds:uri="6cc8ca2e-56d8-406d-8e41-68c6b727753a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>